<commit_message>
feat: import data from excel without image
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -50,12 +52,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,13 +542,25 @@
           <t>创建者</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>创建时间</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>修改时间</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="180" customHeight="1">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>数学</t>
+        </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -557,7 +574,11 @@
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
@@ -567,8 +588,10 @@
       <c r="I2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>3</v>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
       </c>
       <c r="K2" s="2" t="b">
         <v>1</v>
@@ -585,6 +608,12 @@
         <is>
           <t>ben</t>
         </is>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>45219</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>45222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: generate exam without images
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,7 +844,7 @@
     </row>
     <row r="7" ht="180" customHeight="1">
       <c r="A7" s="2" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
@@ -854,7 +854,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr"/>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -862,7 +866,11 @@
         </is>
       </c>
       <c r="F7" s="2" t="n"/>
-      <c r="G7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H7" s="2" t="b">
         <v>1</v>
       </c>
@@ -902,7 +910,7 @@
     </row>
     <row r="8" ht="180" customHeight="1">
       <c r="A8" s="2" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
@@ -912,7 +920,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -920,7 +932,11 @@
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
-      <c r="G8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H8" s="2" t="b">
         <v>1</v>
       </c>
@@ -960,7 +976,7 @@
     </row>
     <row r="9" ht="180" customHeight="1">
       <c r="A9" s="2" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
@@ -982,11 +998,7 @@
         </is>
       </c>
       <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G9" s="2" t="inlineStr"/>
       <c r="H9" s="2" t="b">
         <v>1</v>
       </c>
@@ -1026,7 +1038,7 @@
     </row>
     <row r="10" ht="180" customHeight="1">
       <c r="A10" s="2" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
@@ -1048,11 +1060,7 @@
         </is>
       </c>
       <c r="F10" s="2" t="n"/>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G10" s="2" t="inlineStr"/>
       <c r="H10" s="2" t="b">
         <v>1</v>
       </c>
@@ -1092,7 +1100,7 @@
     </row>
     <row r="11" ht="180" customHeight="1">
       <c r="A11" s="2" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
@@ -1154,7 +1162,7 @@
     </row>
     <row r="12" ht="180" customHeight="1">
       <c r="A12" s="2" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
@@ -1216,7 +1224,7 @@
     </row>
     <row r="13" ht="180" customHeight="1">
       <c r="A13" s="2" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
@@ -1278,7 +1286,7 @@
     </row>
     <row r="14" ht="180" customHeight="1">
       <c r="A14" s="2" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
@@ -1340,7 +1348,7 @@
     </row>
     <row r="15" ht="180" customHeight="1">
       <c r="A15" s="2" t="n">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
@@ -1350,7 +1358,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr"/>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -1398,7 +1410,7 @@
     </row>
     <row r="16" ht="180" customHeight="1">
       <c r="A16" s="2" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>1</v>
@@ -1408,7 +1420,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr"/>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -1456,7 +1472,7 @@
     </row>
     <row r="17" ht="180" customHeight="1">
       <c r="A17" s="2" t="n">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
@@ -1478,7 +1494,11 @@
         </is>
       </c>
       <c r="F17" s="2" t="n"/>
-      <c r="G17" s="2" t="inlineStr"/>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H17" s="2" t="b">
         <v>1</v>
       </c>
@@ -1518,7 +1538,7 @@
     </row>
     <row r="18" ht="180" customHeight="1">
       <c r="A18" s="2" t="n">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>1</v>
@@ -1580,7 +1600,7 @@
     </row>
     <row r="19" ht="180" customHeight="1">
       <c r="A19" s="2" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>1</v>
@@ -1642,7 +1662,7 @@
     </row>
     <row r="20" ht="180" customHeight="1">
       <c r="A20" s="2" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>1</v>
@@ -1704,7 +1724,7 @@
     </row>
     <row r="21" ht="180" customHeight="1">
       <c r="A21" s="2" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>1</v>
@@ -1714,7 +1734,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr"/>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -1762,7 +1786,7 @@
     </row>
     <row r="22" ht="180" customHeight="1">
       <c r="A22" s="2" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>1</v>
@@ -1772,7 +1796,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr"/>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -1780,7 +1808,11 @@
         </is>
       </c>
       <c r="F22" s="2" t="n"/>
-      <c r="G22" s="2" t="inlineStr"/>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H22" s="2" t="b">
         <v>1</v>
       </c>
@@ -1820,7 +1852,7 @@
     </row>
     <row r="23" ht="180" customHeight="1">
       <c r="A23" s="2" t="n">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>1</v>
@@ -1886,7 +1918,7 @@
     </row>
     <row r="24" ht="180" customHeight="1">
       <c r="A24" s="2" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>1</v>
@@ -1948,7 +1980,7 @@
     </row>
     <row r="25" ht="180" customHeight="1">
       <c r="A25" s="2" t="n">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>1</v>
@@ -2010,7 +2042,7 @@
     </row>
     <row r="26" ht="180" customHeight="1">
       <c r="A26" s="2" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>1</v>
@@ -2072,7 +2104,7 @@
     </row>
     <row r="27" ht="180" customHeight="1">
       <c r="A27" s="2" t="n">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>1</v>
@@ -2134,7 +2166,7 @@
     </row>
     <row r="28" ht="180" customHeight="1">
       <c r="A28" s="2" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>1</v>
@@ -2144,7 +2176,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D28" s="2" t="inlineStr"/>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -2192,7 +2228,7 @@
     </row>
     <row r="29" ht="180" customHeight="1">
       <c r="A29" s="2" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>1</v>
@@ -2202,7 +2238,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -2250,7 +2290,7 @@
     </row>
     <row r="30" ht="180" customHeight="1">
       <c r="A30" s="2" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>1</v>
@@ -2272,11 +2312,7 @@
         </is>
       </c>
       <c r="F30" s="2" t="n"/>
-      <c r="G30" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G30" s="2" t="inlineStr"/>
       <c r="H30" s="2" t="b">
         <v>1</v>
       </c>
@@ -2316,7 +2352,7 @@
     </row>
     <row r="31" ht="180" customHeight="1">
       <c r="A31" s="2" t="n">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>1</v>
@@ -2338,11 +2374,7 @@
         </is>
       </c>
       <c r="F31" s="2" t="n"/>
-      <c r="G31" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G31" s="2" t="inlineStr"/>
       <c r="H31" s="2" t="b">
         <v>1</v>
       </c>
@@ -2382,7 +2414,7 @@
     </row>
     <row r="32" ht="180" customHeight="1">
       <c r="A32" s="2" t="n">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1</v>
@@ -2404,7 +2436,11 @@
         </is>
       </c>
       <c r="F32" s="2" t="n"/>
-      <c r="G32" s="2" t="inlineStr"/>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H32" s="2" t="b">
         <v>1</v>
       </c>
@@ -2444,7 +2480,7 @@
     </row>
     <row r="33" ht="180" customHeight="1">
       <c r="A33" s="2" t="n">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>1</v>
@@ -2506,7 +2542,7 @@
     </row>
     <row r="34" ht="180" customHeight="1">
       <c r="A34" s="2" t="n">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>1</v>
@@ -2568,7 +2604,7 @@
     </row>
     <row r="35" ht="180" customHeight="1">
       <c r="A35" s="2" t="n">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>1</v>
@@ -2630,7 +2666,7 @@
     </row>
     <row r="36" ht="180" customHeight="1">
       <c r="A36" s="2" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>1</v>
@@ -2640,7 +2676,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr"/>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -2688,7 +2728,7 @@
     </row>
     <row r="37" ht="180" customHeight="1">
       <c r="A37" s="2" t="n">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1</v>
@@ -2698,7 +2738,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D37" s="2" t="inlineStr"/>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -2706,7 +2750,11 @@
         </is>
       </c>
       <c r="F37" s="2" t="n"/>
-      <c r="G37" s="2" t="inlineStr"/>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H37" s="2" t="b">
         <v>1</v>
       </c>
@@ -2746,7 +2794,7 @@
     </row>
     <row r="38" ht="180" customHeight="1">
       <c r="A38" s="2" t="n">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>1</v>
@@ -2768,7 +2816,11 @@
         </is>
       </c>
       <c r="F38" s="2" t="n"/>
-      <c r="G38" s="2" t="inlineStr"/>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H38" s="2" t="b">
         <v>1</v>
       </c>
@@ -2808,7 +2860,7 @@
     </row>
     <row r="39" ht="180" customHeight="1">
       <c r="A39" s="2" t="n">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>1</v>
@@ -2870,7 +2922,7 @@
     </row>
     <row r="40" ht="180" customHeight="1">
       <c r="A40" s="2" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>1</v>
@@ -2932,7 +2984,7 @@
     </row>
     <row r="41" ht="180" customHeight="1">
       <c r="A41" s="2" t="n">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>1</v>
@@ -2994,7 +3046,7 @@
     </row>
     <row r="42" ht="180" customHeight="1">
       <c r="A42" s="2" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>1</v>
@@ -3004,7 +3056,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr"/>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -3052,7 +3108,7 @@
     </row>
     <row r="43" ht="180" customHeight="1">
       <c r="A43" s="2" t="n">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>1</v>
@@ -3062,7 +3118,11 @@
           <t>数学</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr"/>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>看图填数</t>
+        </is>
+      </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
           <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
@@ -3110,7 +3170,7 @@
     </row>
     <row r="44" ht="180" customHeight="1">
       <c r="A44" s="2" t="n">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
@@ -3132,11 +3192,7 @@
         </is>
       </c>
       <c r="F44" s="2" t="n"/>
-      <c r="G44" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G44" s="2" t="inlineStr"/>
       <c r="H44" s="2" t="b">
         <v>1</v>
       </c>
@@ -3176,7 +3232,7 @@
     </row>
     <row r="45" ht="180" customHeight="1">
       <c r="A45" s="2" t="n">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1</v>
@@ -3238,7 +3294,7 @@
     </row>
     <row r="46" ht="180" customHeight="1">
       <c r="A46" s="2" t="n">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>1</v>
@@ -3295,1106 +3351,6 @@
         <v>45222</v>
       </c>
       <c r="Q46" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="47" ht="180" customHeight="1">
-      <c r="A47" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D47" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E47" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F47" s="2" t="n"/>
-      <c r="G47" s="2" t="inlineStr"/>
-      <c r="H47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K47" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M47" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O47" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P47" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q47" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="48" ht="180" customHeight="1">
-      <c r="A48" s="2" t="n">
-        <v>94</v>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D48" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E48" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F48" s="2" t="n"/>
-      <c r="G48" s="2" t="inlineStr"/>
-      <c r="H48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J48" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K48" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M48" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O48" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P48" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q48" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="49" ht="180" customHeight="1">
-      <c r="A49" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D49" s="2" t="inlineStr"/>
-      <c r="E49" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F49" s="2" t="n"/>
-      <c r="G49" s="2" t="inlineStr"/>
-      <c r="H49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J49" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K49" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M49" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O49" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P49" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q49" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="50" ht="180" customHeight="1">
-      <c r="A50" s="2" t="n">
-        <v>96</v>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D50" s="2" t="inlineStr"/>
-      <c r="E50" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F50" s="2" t="n"/>
-      <c r="G50" s="2" t="inlineStr"/>
-      <c r="H50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K50" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O50" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P50" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q50" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="51" ht="180" customHeight="1">
-      <c r="A51" s="2" t="n">
-        <v>97</v>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D51" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E51" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F51" s="2" t="n"/>
-      <c r="G51" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
-      <c r="H51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I51" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J51" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K51" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M51" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O51" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P51" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q51" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="52" ht="180" customHeight="1">
-      <c r="A52" s="2" t="n">
-        <v>98</v>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D52" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E52" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F52" s="2" t="n"/>
-      <c r="G52" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
-      <c r="H52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J52" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K52" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M52" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O52" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P52" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q52" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="53" ht="180" customHeight="1">
-      <c r="A53" s="2" t="n">
-        <v>99</v>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D53" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E53" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F53" s="2" t="n"/>
-      <c r="G53" s="2" t="inlineStr"/>
-      <c r="H53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I53" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J53" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K53" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M53" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N53" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O53" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P53" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q53" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="54" ht="180" customHeight="1">
-      <c r="A54" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D54" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E54" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F54" s="2" t="n"/>
-      <c r="G54" s="2" t="inlineStr"/>
-      <c r="H54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I54" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J54" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K54" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M54" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O54" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P54" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q54" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="55" ht="180" customHeight="1">
-      <c r="A55" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D55" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E55" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F55" s="2" t="n"/>
-      <c r="G55" s="2" t="inlineStr"/>
-      <c r="H55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I55" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J55" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K55" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M55" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P55" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q55" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="56" ht="180" customHeight="1">
-      <c r="A56" s="2" t="n">
-        <v>102</v>
-      </c>
-      <c r="B56" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D56" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E56" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F56" s="2" t="n"/>
-      <c r="G56" s="2" t="inlineStr"/>
-      <c r="H56" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I56" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J56" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K56" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L56" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N56" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P56" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q56" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="57" ht="180" customHeight="1">
-      <c r="A57" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D57" s="2" t="inlineStr"/>
-      <c r="E57" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F57" s="2" t="n"/>
-      <c r="G57" s="2" t="inlineStr"/>
-      <c r="H57" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I57" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J57" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K57" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L57" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M57" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N57" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O57" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P57" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q57" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="58" ht="180" customHeight="1">
-      <c r="A58" s="2" t="n">
-        <v>104</v>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D58" s="2" t="inlineStr"/>
-      <c r="E58" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F58" s="2" t="n"/>
-      <c r="G58" s="2" t="inlineStr"/>
-      <c r="H58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I58" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J58" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K58" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M58" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O58" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P58" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q58" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="59" ht="180" customHeight="1">
-      <c r="A59" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="B59" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D59" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E59" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F59" s="2" t="n"/>
-      <c r="G59" s="2" t="inlineStr"/>
-      <c r="H59" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I59" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J59" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K59" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L59" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M59" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N59" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O59" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P59" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q59" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="60" ht="180" customHeight="1">
-      <c r="A60" s="2" t="n">
-        <v>106</v>
-      </c>
-      <c r="B60" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D60" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E60" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F60" s="2" t="n"/>
-      <c r="G60" s="2" t="inlineStr"/>
-      <c r="H60" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I60" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J60" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K60" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L60" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M60" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N60" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O60" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P60" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q60" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="61" ht="180" customHeight="1">
-      <c r="A61" s="2" t="n">
-        <v>107</v>
-      </c>
-      <c r="B61" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C61" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D61" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E61" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F61" s="2" t="n"/>
-      <c r="G61" s="2" t="inlineStr"/>
-      <c r="H61" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I61" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K61" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L61" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M61" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N61" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O61" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P61" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q61" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="62" ht="180" customHeight="1">
-      <c r="A62" s="2" t="n">
-        <v>108</v>
-      </c>
-      <c r="B62" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C62" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D62" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E62" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F62" s="2" t="n"/>
-      <c r="G62" s="2" t="inlineStr"/>
-      <c r="H62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I62" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K62" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M62" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O62" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P62" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q62" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="63" ht="180" customHeight="1">
-      <c r="A63" s="2" t="n">
-        <v>109</v>
-      </c>
-      <c r="B63" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D63" s="2" t="inlineStr"/>
-      <c r="E63" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F63" s="2" t="n"/>
-      <c r="G63" s="2" t="inlineStr"/>
-      <c r="H63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J63" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K63" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M63" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O63" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P63" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q63" s="3" t="n">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="64" ht="180" customHeight="1">
-      <c r="A64" s="2" t="n">
-        <v>110</v>
-      </c>
-      <c r="B64" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="inlineStr"/>
-      <c r="E64" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F64" s="2" t="n"/>
-      <c r="G64" s="2" t="inlineStr"/>
-      <c r="H64" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I64" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K64" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L64" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M64" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N64" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O64" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="P64" s="3" t="n">
-        <v>45222</v>
-      </c>
-      <c r="Q64" s="3" t="n">
         <v>45222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add picture to docx
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -137,6 +137,61 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4743450" cy="1724025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>45</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4743450" cy="1724025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,7 +585,7 @@
     </row>
     <row r="2" ht="180" customHeight="1">
       <c r="A2" s="2" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1</v>
@@ -552,11 +607,7 @@
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="inlineStr"/>
       <c r="H2" s="2" t="b">
         <v>1</v>
       </c>
@@ -596,7 +647,7 @@
     </row>
     <row r="3" ht="180" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1</v>
@@ -658,7 +709,7 @@
     </row>
     <row r="4" ht="180" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -720,7 +771,7 @@
     </row>
     <row r="5" ht="180" customHeight="1">
       <c r="A5" s="2" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
@@ -782,7 +833,7 @@
     </row>
     <row r="6" ht="180" customHeight="1">
       <c r="A6" s="2" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
@@ -804,7 +855,11 @@
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
-      <c r="G6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H6" s="2" t="b">
         <v>1</v>
       </c>
@@ -844,7 +899,7 @@
     </row>
     <row r="7" ht="180" customHeight="1">
       <c r="A7" s="2" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
@@ -910,7 +965,7 @@
     </row>
     <row r="8" ht="180" customHeight="1">
       <c r="A8" s="2" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
@@ -932,11 +987,7 @@
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G8" s="2" t="inlineStr"/>
       <c r="H8" s="2" t="b">
         <v>1</v>
       </c>
@@ -976,7 +1027,7 @@
     </row>
     <row r="9" ht="180" customHeight="1">
       <c r="A9" s="2" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
@@ -1038,7 +1089,7 @@
     </row>
     <row r="10" ht="180" customHeight="1">
       <c r="A10" s="2" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
@@ -1100,7 +1151,7 @@
     </row>
     <row r="11" ht="180" customHeight="1">
       <c r="A11" s="2" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
@@ -1162,7 +1213,7 @@
     </row>
     <row r="12" ht="180" customHeight="1">
       <c r="A12" s="2" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
@@ -1224,7 +1275,7 @@
     </row>
     <row r="13" ht="180" customHeight="1">
       <c r="A13" s="2" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
@@ -1286,7 +1337,7 @@
     </row>
     <row r="14" ht="180" customHeight="1">
       <c r="A14" s="2" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
@@ -1348,7 +1399,7 @@
     </row>
     <row r="15" ht="180" customHeight="1">
       <c r="A15" s="2" t="n">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
@@ -1365,12 +1416,16 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
+          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
 (2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
         </is>
       </c>
       <c r="F15" s="2" t="n"/>
-      <c r="G15" s="2" t="inlineStr"/>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H15" s="2" t="b">
         <v>1</v>
       </c>
@@ -3311,7 +3366,7 @@
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
+          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
 (2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
         </is>
       </c>
@@ -3356,5 +3411,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add answer field
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -483,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,7 @@
     <col width="50" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
+    <row r="1" ht="50" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
@@ -574,20 +574,25 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>答案&amp;解题思路</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>是否发布</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>创建者</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>创建时间</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>修改时间</t>
         </is>
@@ -643,18 +648,23 @@
           <t>202cb962ac59075b964b07152d234b70</t>
         </is>
       </c>
-      <c r="P2" s="2" t="b">
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>1,2,3</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="R2" s="2" t="inlineStr">
         <is>
           <t>ben</t>
         </is>
       </c>
-      <c r="R2" s="3" t="n">
+      <c r="S2" s="3" t="n">
         <v>45223</v>
       </c>
-      <c r="S2" s="3" t="n">
+      <c r="T2" s="3" t="n">
         <v>45223</v>
       </c>
     </row>
@@ -710,25 +720,26 @@
         </is>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
           <t>daf2fe1cc1b294de547d7e45ad932567</t>
         </is>
       </c>
-      <c r="P3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="2" t="inlineStr">
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
         <is>
           <t>ben</t>
         </is>
       </c>
-      <c r="R3" s="3" t="n">
+      <c r="S3" s="3" t="n">
         <v>45222</v>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="T3" s="3" t="n">
         <v>45223</v>
       </c>
     </row>
@@ -780,25 +791,26 @@
         </is>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
           <t>1cea746e2b436ad83bb15df6868ba92c</t>
         </is>
       </c>
-      <c r="P4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2" t="inlineStr">
+      <c r="P4" s="2" t="n"/>
+      <c r="Q4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="inlineStr">
         <is>
           <t>ben</t>
         </is>
       </c>
-      <c r="R4" s="3" t="n">
+      <c r="S4" s="3" t="n">
         <v>45222</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="T4" s="3" t="n">
         <v>45223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: read image from excel to admin
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -170,7 +170,7 @@
     <from>
       <col>5</col>
       <colOff>0</colOff>
-      <row>3</row>
+      <row>4</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="4743450" cy="1724025"/>
@@ -483,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,7 @@
     <col width="50" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50" customHeight="1">
+    <row r="1" ht="60" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id</t>
@@ -600,28 +600,33 @@
     </row>
     <row r="2" ht="180" customHeight="1">
       <c r="A2" s="2" t="n">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>数学</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>看图填数</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
+(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="b">
         <v>1</v>
       </c>
@@ -633,28 +638,32 @@
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>未分类</t>
+          <t>看图填数</t>
         </is>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="n"/>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>小学数学单元过关练习</t>
+        </is>
+      </c>
       <c r="N2" s="2" t="n">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>202cb962ac59075b964b07152d234b70</t>
+          <t>daf2fe1cc1b294de547d7e45ad932567</t>
         </is>
       </c>
       <c r="P2" s="2" t="inlineStr">
         <is>
-          <t>1,2,3</t>
+          <t>4,5,6</t>
         </is>
       </c>
       <c r="Q2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -670,7 +679,7 @@
     </row>
     <row r="3" ht="180" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1</v>
@@ -692,11 +701,7 @@
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G3" s="2" t="inlineStr"/>
       <c r="H3" s="2" t="b">
         <v>1</v>
       </c>
@@ -720,14 +725,18 @@
         </is>
       </c>
       <c r="N3" s="2" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>daf2fe1cc1b294de547d7e45ad932567</t>
-        </is>
-      </c>
-      <c r="P3" s="2" t="n"/>
+          <t>7c7972d70c830a9300b2f3be0c838a72</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>1,2,3</t>
+        </is>
+      </c>
       <c r="Q3" s="2" t="b">
         <v>1</v>
       </c>
@@ -737,7 +746,7 @@
         </is>
       </c>
       <c r="S3" s="3" t="n">
-        <v>45222</v>
+        <v>45223</v>
       </c>
       <c r="T3" s="3" t="n">
         <v>45223</v>
@@ -745,7 +754,7 @@
     </row>
     <row r="4" ht="180" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -757,15 +766,10 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
+          <t>test123</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="n"/>
       <c r="G4" s="2" t="inlineStr"/>
       <c r="H4" s="2" t="b">
@@ -779,26 +783,22 @@
       </c>
       <c r="K4" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
+          <t>未分类</t>
         </is>
       </c>
       <c r="L4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
+      <c r="M4" s="2" t="inlineStr"/>
       <c r="N4" s="2" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
-          <t>1cea746e2b436ad83bb15df6868ba92c</t>
-        </is>
-      </c>
-      <c r="P4" s="2" t="n"/>
+          <t>d41d8cd98f00b204e9800998ecf8427e</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr"/>
       <c r="Q4" s="2" t="b">
         <v>1</v>
       </c>
@@ -808,9 +808,79 @@
         </is>
       </c>
       <c r="S4" s="3" t="n">
-        <v>45222</v>
+        <v>45223</v>
       </c>
       <c r="T4" s="3" t="n">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="5" ht="180" customHeight="1">
+      <c r="A5" s="2" t="n">
+        <v>141</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>英语</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="inlineStr"/>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>未分类</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>8f2acdcbe52f06a042904069ef9310a8</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>1,2,3</t>
+        </is>
+      </c>
+      <c r="Q5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>ben</t>
+        </is>
+      </c>
+      <c r="S5" s="3" t="n">
+        <v>45223</v>
+      </c>
+      <c r="T5" s="3" t="n">
         <v>45223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: spilit views to specific view file
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -145,7 +145,7 @@
     <from>
       <col>5</col>
       <colOff>0</colOff>
-      <row>2</row>
+      <row>1</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="4743450" cy="1724025"/>
@@ -170,7 +170,7 @@
     <from>
       <col>5</col>
       <colOff>0</colOff>
-      <row>4</row>
+      <row>3</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="4743450" cy="1724025"/>
@@ -181,6 +181,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4743450" cy="1724025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -600,33 +625,28 @@
     </row>
     <row r="2" ht="180" customHeight="1">
       <c r="A2" s="2" t="n">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>数学</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
+          <t>test</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
+          <t>123</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="inlineStr"/>
       <c r="H2" s="2" t="b">
         <v>1</v>
       </c>
@@ -638,32 +658,28 @@
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
+          <t>未分类</t>
         </is>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
+      <c r="M2" s="2" t="inlineStr"/>
       <c r="N2" s="2" t="n">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>daf2fe1cc1b294de547d7e45ad932567</t>
+          <t>7c74d2bfd53207083875d8908eb08544</t>
         </is>
       </c>
       <c r="P2" s="2" t="inlineStr">
         <is>
-          <t>4,5,6</t>
+          <t>1,2,3</t>
         </is>
       </c>
       <c r="Q2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -679,7 +695,7 @@
     </row>
     <row r="3" ht="180" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1</v>
@@ -696,12 +712,16 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
+          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
 (2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>图片下方描述111</t>
+        </is>
+      </c>
       <c r="H3" s="2" t="b">
         <v>1</v>
       </c>
@@ -725,16 +745,16 @@
         </is>
       </c>
       <c r="N3" s="2" t="n">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>7c7972d70c830a9300b2f3be0c838a72</t>
+          <t>856a24128051fad580b980bfe410d0f3</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>1,2,3</t>
+          <t>4,5,6</t>
         </is>
       </c>
       <c r="Q3" s="2" t="b">
@@ -754,7 +774,7 @@
     </row>
     <row r="4" ht="180" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -791,7 +811,7 @@
       </c>
       <c r="M4" s="2" t="inlineStr"/>
       <c r="N4" s="2" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
@@ -816,24 +836,25 @@
     </row>
     <row r="5" ht="180" customHeight="1">
       <c r="A5" s="2" t="n">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>英语</t>
+          <t>数学</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>看图填数</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
+(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -849,19 +870,23 @@
       </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>未分类</t>
+          <t>看图填数</t>
         </is>
       </c>
       <c r="L5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="2" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>小学数学单元过关练习</t>
+        </is>
+      </c>
       <c r="N5" s="2" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O5" s="2" t="inlineStr">
         <is>
-          <t>8f2acdcbe52f06a042904069ef9310a8</t>
+          <t>d003a87b7c21f754e1dad940f522ddf0</t>
         </is>
       </c>
       <c r="P5" s="2" t="inlineStr">
@@ -870,7 +895,7 @@
         </is>
       </c>
       <c r="Q5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat: export to excel by conditions
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -145,7 +145,7 @@
     <from>
       <col>5</col>
       <colOff>0</colOff>
-      <row>1</row>
+      <row>2</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="4743450" cy="1724025"/>
@@ -156,56 +156,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>3</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="4743450" cy="1724025"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>4</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="4743450" cy="1724025"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -508,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,7 +575,7 @@
     </row>
     <row r="2" ht="180" customHeight="1">
       <c r="A2" s="2" t="n">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1</v>
@@ -637,14 +587,10 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
+          <t>yingyu</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr"/>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="inlineStr"/>
       <c r="H2" s="2" t="b">
@@ -664,22 +610,18 @@
       <c r="L2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="inlineStr"/>
+      <c r="M2" s="2" t="n"/>
       <c r="N2" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>7c74d2bfd53207083875d8908eb08544</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr">
-        <is>
-          <t>1,2,3</t>
-        </is>
-      </c>
+          <t>d41d8cd98f00b204e9800998ecf8427e</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr"/>
       <c r="Q2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -695,33 +637,28 @@
     </row>
     <row r="3" ht="180" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>数学</t>
+          <t>英语</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
+          <t>test</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
+          <t>123</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>图片下方描述111</t>
-        </is>
-      </c>
+      <c r="G3" s="2" t="inlineStr"/>
       <c r="H3" s="2" t="b">
         <v>1</v>
       </c>
@@ -733,32 +670,28 @@
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>看图填数</t>
+          <t>未分类</t>
         </is>
       </c>
       <c r="L3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
+      <c r="M3" s="2" t="inlineStr"/>
       <c r="N3" s="2" t="n">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>856a24128051fad580b980bfe410d0f3</t>
+          <t>7c74d2bfd53207083875d8908eb08544</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>4,5,6</t>
+          <t>1,2,3</t>
         </is>
       </c>
       <c r="Q3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="2" t="inlineStr">
         <is>
@@ -769,143 +702,6 @@
         <v>45223</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>45223</v>
-      </c>
-    </row>
-    <row r="4" ht="180" customHeight="1">
-      <c r="A4" s="2" t="n">
-        <v>165</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>test123</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="inlineStr"/>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>未分类</t>
-        </is>
-      </c>
-      <c r="L4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2" t="inlineStr"/>
-      <c r="N4" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="O4" s="2" t="inlineStr">
-        <is>
-          <t>d41d8cd98f00b204e9800998ecf8427e</t>
-        </is>
-      </c>
-      <c r="P4" s="2" t="inlineStr"/>
-      <c r="Q4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="S4" s="3" t="n">
-        <v>45223</v>
-      </c>
-      <c r="T4" s="3" t="n">
-        <v>45223</v>
-      </c>
-    </row>
-    <row r="5" ht="180" customHeight="1">
-      <c r="A5" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>(1) 小动物们排成一排，从右边数，小猴子排在第3个，这一排小动物共有 (        ) 个，被挡住的小动物有 (        ) 个。
-(2) 最左边的2个小动物排到队友的最右边后，从左边数，小猴子排在第 (        ) 个，它回家后，还有 (        ) 个小动物。</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="n"/>
-      <c r="G5" s="2" t="inlineStr"/>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>看图填数</t>
-        </is>
-      </c>
-      <c r="L5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
-        <is>
-          <t>小学数学单元过关练习</t>
-        </is>
-      </c>
-      <c r="N5" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="O5" s="2" t="inlineStr">
-        <is>
-          <t>d003a87b7c21f754e1dad940f522ddf0</t>
-        </is>
-      </c>
-      <c r="P5" s="2" t="inlineStr">
-        <is>
-          <t>1,2,3</t>
-        </is>
-      </c>
-      <c r="Q5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="S5" s="3" t="n">
-        <v>45223</v>
-      </c>
-      <c r="T5" s="3" t="n">
         <v>45223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: save excel when no data
</commit_message>
<xml_diff>
--- a/media/study/files/output.xlsx
+++ b/media/study/files/output.xlsx
@@ -16,20 +16,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,17 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -137,36 +122,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>2</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="4743450" cy="1724025"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,255 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="80" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="60" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>年级</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>学科</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>标题</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>图片上方描述</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>图片</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>图片下方描述</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>是否课内习题</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>分数</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>出错次数</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>题目类型</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>是否固定题</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>出自哪个试卷</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>出题次数</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>MD5值</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>答案&amp;解题思路</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>是否发布</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>创建者</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>创建时间</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>修改时间</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="180" customHeight="1">
-      <c r="A2" s="2" t="n">
-        <v>167</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>英语</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>yingyu</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="inlineStr"/>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>未分类</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="n"/>
-      <c r="N2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>d41d8cd98f00b204e9800998ecf8427e</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr"/>
-      <c r="Q2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="S2" s="3" t="n">
-        <v>45223</v>
-      </c>
-      <c r="T2" s="3" t="n">
-        <v>45223</v>
-      </c>
-    </row>
-    <row r="3" ht="180" customHeight="1">
-      <c r="A3" s="2" t="n">
-        <v>163</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>英语</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="inlineStr"/>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>未分类</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2" t="inlineStr"/>
-      <c r="N3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2" t="inlineStr">
-        <is>
-          <t>7c74d2bfd53207083875d8908eb08544</t>
-        </is>
-      </c>
-      <c r="P3" s="2" t="inlineStr">
-        <is>
-          <t>1,2,3</t>
-        </is>
-      </c>
-      <c r="Q3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2" t="inlineStr">
-        <is>
-          <t>ben</t>
-        </is>
-      </c>
-      <c r="S3" s="3" t="n">
-        <v>45223</v>
-      </c>
-      <c r="T3" s="3" t="n">
-        <v>45223</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>